<commit_message>
Analysis of results from 20180325
</commit_message>
<xml_diff>
--- a/format_aggregate_results.xlsx
+++ b/format_aggregate_results.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="14900" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="15360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="Paper_AggregateData" localSheetId="0">Sheet1!$A$1:$F$13</definedName>
+    <definedName name="Paper_AggregateData_1" localSheetId="0">Sheet1!$A$15:$F$27</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -32,7 +33,19 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="Paper_AggregateData" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/jdimas/GitHub/ABMNK/20180324_data/Paper_AggregateData.csv" tab="0" comma="1">
+    <textPr fileType="mac" sourceFile="/Users/jdimas/GitHub/ABMNK/20180324_data/Paper_AggregateData.csv" tab="0" comma="1">
+      <textFields count="6">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="Paper_AggregateData1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/jdimas/GitHub/ABMNK/20180325_data/Paper_AggregateData.csv" comma="1">
       <textFields count="6">
         <textField/>
         <textField/>
@@ -47,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="24">
   <si>
     <t>sce_1</t>
   </si>
@@ -126,7 +139,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -167,11 +180,11 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -190,6 +203,10 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Paper_AggregateData_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Paper_AggregateData" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -456,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="E3" zoomScale="150" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -573,7 +590,7 @@
         <v>(0.0181)</v>
       </c>
       <c r="J3" s="2" t="str">
-        <f t="shared" ref="J3:M3" si="1">"("&amp;TRUNC(C3,4)&amp;")"</f>
+        <f t="shared" ref="J3:K3" si="1">"("&amp;TRUNC(C3,4)&amp;")"</f>
         <v>(0.0588)</v>
       </c>
       <c r="K3" s="2" t="str">
@@ -986,10 +1003,526 @@
       </c>
       <c r="I13" s="4"/>
     </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="2" t="str">
+        <f>B15</f>
+        <v>sce_1</v>
+      </c>
+      <c r="J15" s="2" t="str">
+        <f t="shared" ref="J15:J16" si="11">C15</f>
+        <v>sce_2</v>
+      </c>
+      <c r="K15" s="2" t="str">
+        <f t="shared" ref="K15:K16" si="12">D15</f>
+        <v>sce_3</v>
+      </c>
+      <c r="L15" s="2" t="str">
+        <f t="shared" ref="L15:L16" si="13">E15</f>
+        <v>sce_4</v>
+      </c>
+      <c r="M15" s="2" t="str">
+        <f t="shared" ref="M15:M16" si="14">F15</f>
+        <v>sce_5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>4.1331675080256702E-3</v>
+      </c>
+      <c r="C16">
+        <v>1.2268855776419001E-2</v>
+      </c>
+      <c r="D16">
+        <v>4.2179959032307597E-3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="3">
+        <f>B16</f>
+        <v>4.1331675080256702E-3</v>
+      </c>
+      <c r="J16" s="3">
+        <f t="shared" si="11"/>
+        <v>1.2268855776419001E-2</v>
+      </c>
+      <c r="K16" s="3">
+        <f t="shared" si="12"/>
+        <v>4.2179959032307597E-3</v>
+      </c>
+      <c r="L16" s="3" t="str">
+        <f t="shared" si="13"/>
+        <v>NA</v>
+      </c>
+      <c r="M16" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17">
+        <v>1.8432551047843301E-2</v>
+      </c>
+      <c r="C17">
+        <v>4.2944296182704698E-2</v>
+      </c>
+      <c r="D17">
+        <v>1.8419498351666001E-2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="2" t="str">
+        <f>"("&amp;TRUNC(B17,4)&amp;")"</f>
+        <v>(0.0184)</v>
+      </c>
+      <c r="J17" s="2" t="str">
+        <f t="shared" ref="J17" si="15">"("&amp;TRUNC(C17,4)&amp;")"</f>
+        <v>(0.0429)</v>
+      </c>
+      <c r="K17" s="2" t="str">
+        <f t="shared" ref="K17" si="16">"("&amp;TRUNC(D17,4)&amp;")"</f>
+        <v>(0.0184)</v>
+      </c>
+      <c r="L17" s="2" t="str">
+        <f>E17</f>
+        <v>NA</v>
+      </c>
+      <c r="M17" s="2" t="str">
+        <f>F17</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>2.1721468844569401E-2</v>
+      </c>
+      <c r="C18">
+        <v>2.50659129017058E-2</v>
+      </c>
+      <c r="D18">
+        <v>1.8931396216324E-2</v>
+      </c>
+      <c r="E18">
+        <v>6.3319080692315899E-2</v>
+      </c>
+      <c r="F18">
+        <v>0.459863208058088</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" s="3">
+        <f>B18</f>
+        <v>2.1721468844569401E-2</v>
+      </c>
+      <c r="J18" s="3">
+        <f t="shared" ref="J18" si="17">C18</f>
+        <v>2.50659129017058E-2</v>
+      </c>
+      <c r="K18" s="3">
+        <f t="shared" ref="K18" si="18">D18</f>
+        <v>1.8931396216324E-2</v>
+      </c>
+      <c r="L18" s="3">
+        <f t="shared" ref="L18" si="19">E18</f>
+        <v>6.3319080692315899E-2</v>
+      </c>
+      <c r="M18" s="3">
+        <f t="shared" ref="M18" si="20">F18</f>
+        <v>0.459863208058088</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <v>3.93052846143589E-2</v>
+      </c>
+      <c r="C19">
+        <v>5.8645193983012302E-2</v>
+      </c>
+      <c r="D19">
+        <v>2.4709924042835101E-2</v>
+      </c>
+      <c r="E19">
+        <v>0.201286816453108</v>
+      </c>
+      <c r="F19">
+        <v>0.44798123174654503</v>
+      </c>
+      <c r="I19" s="2" t="str">
+        <f>"("&amp;TRUNC(B19,4)&amp;")"</f>
+        <v>(0.0393)</v>
+      </c>
+      <c r="J19" s="2" t="str">
+        <f t="shared" ref="J19" si="21">"("&amp;TRUNC(C19,4)&amp;")"</f>
+        <v>(0.0586)</v>
+      </c>
+      <c r="K19" s="2" t="str">
+        <f t="shared" ref="K19" si="22">"("&amp;TRUNC(D19,4)&amp;")"</f>
+        <v>(0.0247)</v>
+      </c>
+      <c r="L19" s="2" t="str">
+        <f t="shared" ref="L19" si="23">"("&amp;TRUNC(E19,4)&amp;")"</f>
+        <v>(0.2012)</v>
+      </c>
+      <c r="M19" s="2" t="str">
+        <f t="shared" ref="M19" si="24">"("&amp;TRUNC(F19,4)&amp;")"</f>
+        <v>(0.4479)</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20">
+        <v>1.1841659487116101</v>
+      </c>
+      <c r="C20">
+        <v>1.1801823179347</v>
+      </c>
+      <c r="D20">
+        <v>1.1937024112580701</v>
+      </c>
+      <c r="E20">
+        <v>1.29130153062804</v>
+      </c>
+      <c r="F20">
+        <v>1.4974706277905201</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" s="3">
+        <f>B20</f>
+        <v>1.1841659487116101</v>
+      </c>
+      <c r="J20" s="3">
+        <f t="shared" ref="J20" si="25">C20</f>
+        <v>1.1801823179347</v>
+      </c>
+      <c r="K20" s="3">
+        <f t="shared" ref="K20" si="26">D20</f>
+        <v>1.1937024112580701</v>
+      </c>
+      <c r="L20" s="3">
+        <f t="shared" ref="L20" si="27">E20</f>
+        <v>1.29130153062804</v>
+      </c>
+      <c r="M20" s="3">
+        <f t="shared" ref="M20" si="28">F20</f>
+        <v>1.4974706277905201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21">
+        <v>0.25767718293840702</v>
+      </c>
+      <c r="C21">
+        <v>0.30441394299351199</v>
+      </c>
+      <c r="D21">
+        <v>0.25708608447272702</v>
+      </c>
+      <c r="E21">
+        <v>0.41469290826098398</v>
+      </c>
+      <c r="F21">
+        <v>0.465912177841799</v>
+      </c>
+      <c r="H21" s="4"/>
+      <c r="I21" s="2" t="str">
+        <f>"("&amp;TRUNC(B21,4)&amp;")"</f>
+        <v>(0.2576)</v>
+      </c>
+      <c r="J21" s="2" t="str">
+        <f t="shared" ref="J21" si="29">"("&amp;TRUNC(C21,4)&amp;")"</f>
+        <v>(0.3044)</v>
+      </c>
+      <c r="K21" s="2" t="str">
+        <f t="shared" ref="K21" si="30">"("&amp;TRUNC(D21,4)&amp;")"</f>
+        <v>(0.257)</v>
+      </c>
+      <c r="L21" s="2" t="str">
+        <f t="shared" ref="L21" si="31">"("&amp;TRUNC(E21,4)&amp;")"</f>
+        <v>(0.4146)</v>
+      </c>
+      <c r="M21" s="2" t="str">
+        <f t="shared" ref="M21" si="32">"("&amp;TRUNC(F21,4)&amp;")"</f>
+        <v>(0.4659)</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22">
+        <v>1.0060490713199299</v>
+      </c>
+      <c r="C22">
+        <v>0.94011846680789901</v>
+      </c>
+      <c r="D22">
+        <v>1.0065881502159399</v>
+      </c>
+      <c r="E22">
+        <v>1.0057138065612301</v>
+      </c>
+      <c r="F22">
+        <v>0.93050894559443598</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="3">
+        <f>B22</f>
+        <v>1.0060490713199299</v>
+      </c>
+      <c r="J22" s="3">
+        <f t="shared" ref="J22" si="33">C22</f>
+        <v>0.94011846680789901</v>
+      </c>
+      <c r="K22" s="3">
+        <f t="shared" ref="K22" si="34">D22</f>
+        <v>1.0065881502159399</v>
+      </c>
+      <c r="L22" s="3">
+        <f t="shared" ref="L22" si="35">E22</f>
+        <v>1.0057138065612301</v>
+      </c>
+      <c r="M22" s="3">
+        <f t="shared" ref="M22" si="36">F22</f>
+        <v>0.93050894559443598</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23">
+        <v>0.132573691356175</v>
+      </c>
+      <c r="C23">
+        <v>0.34572666483862402</v>
+      </c>
+      <c r="D23">
+        <v>0.13644411933887199</v>
+      </c>
+      <c r="E23">
+        <v>0.15992005137642101</v>
+      </c>
+      <c r="F23">
+        <v>0.31129778687931597</v>
+      </c>
+      <c r="I23" s="2" t="str">
+        <f>"("&amp;TRUNC(B23,4)&amp;")"</f>
+        <v>(0.1325)</v>
+      </c>
+      <c r="J23" s="2" t="str">
+        <f t="shared" ref="J23" si="37">"("&amp;TRUNC(C23,4)&amp;")"</f>
+        <v>(0.3457)</v>
+      </c>
+      <c r="K23" s="2" t="str">
+        <f t="shared" ref="K23" si="38">"("&amp;TRUNC(D23,4)&amp;")"</f>
+        <v>(0.1364)</v>
+      </c>
+      <c r="L23" s="2" t="str">
+        <f t="shared" ref="L23" si="39">"("&amp;TRUNC(E23,4)&amp;")"</f>
+        <v>(0.1599)</v>
+      </c>
+      <c r="M23" s="2" t="str">
+        <f t="shared" ref="M23" si="40">"("&amp;TRUNC(F23,4)&amp;")"</f>
+        <v>(0.3112)</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24">
+        <v>4.8883129599792498E-2</v>
+      </c>
+      <c r="C24">
+        <v>4.8565258460957002E-2</v>
+      </c>
+      <c r="D24">
+        <v>4.9112526049179199E-2</v>
+      </c>
+      <c r="E24">
+        <v>4.8534728973367899E-2</v>
+      </c>
+      <c r="F24">
+        <v>4.9941817315470698E-2</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I24" s="3">
+        <f>B24</f>
+        <v>4.8883129599792498E-2</v>
+      </c>
+      <c r="J24" s="3">
+        <f t="shared" ref="J24" si="41">C24</f>
+        <v>4.8565258460957002E-2</v>
+      </c>
+      <c r="K24" s="3">
+        <f t="shared" ref="K24" si="42">D24</f>
+        <v>4.9112526049179199E-2</v>
+      </c>
+      <c r="L24" s="3">
+        <f t="shared" ref="L24" si="43">E24</f>
+        <v>4.8534728973367899E-2</v>
+      </c>
+      <c r="M24" s="3">
+        <f t="shared" ref="M24" si="44">F24</f>
+        <v>4.9941817315470698E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25">
+        <v>1.10559827445223E-2</v>
+      </c>
+      <c r="C25">
+        <v>1.1162973118170201E-2</v>
+      </c>
+      <c r="D25">
+        <v>1.12155799556085E-2</v>
+      </c>
+      <c r="E25">
+        <v>1.1089359493557801E-2</v>
+      </c>
+      <c r="F25">
+        <v>1.11661509679352E-2</v>
+      </c>
+      <c r="I25" s="2" t="str">
+        <f>"("&amp;TRUNC(B25,4)&amp;")"</f>
+        <v>(0.011)</v>
+      </c>
+      <c r="J25" s="2" t="str">
+        <f t="shared" ref="J25" si="45">"("&amp;TRUNC(C25,4)&amp;")"</f>
+        <v>(0.0111)</v>
+      </c>
+      <c r="K25" s="2" t="str">
+        <f t="shared" ref="K25" si="46">"("&amp;TRUNC(D25,4)&amp;")"</f>
+        <v>(0.0112)</v>
+      </c>
+      <c r="L25" s="2" t="str">
+        <f t="shared" ref="L25" si="47">"("&amp;TRUNC(E25,4)&amp;")"</f>
+        <v>(0.011)</v>
+      </c>
+      <c r="M25" s="2" t="str">
+        <f t="shared" ref="M25" si="48">"("&amp;TRUNC(F25,4)&amp;")"</f>
+        <v>(0.0111)</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26">
+        <v>4.9634716282129301E-2</v>
+      </c>
+      <c r="C26">
+        <v>4.9614656724136001E-2</v>
+      </c>
+      <c r="D26">
+        <v>4.99343566095009E-2</v>
+      </c>
+      <c r="E26">
+        <v>4.9655528313587799E-2</v>
+      </c>
+      <c r="F26">
+        <v>5.17825598545422E-2</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I26" s="3">
+        <f>B26</f>
+        <v>4.9634716282129301E-2</v>
+      </c>
+      <c r="J26" s="3">
+        <f t="shared" ref="J26" si="49">C26</f>
+        <v>4.9614656724136001E-2</v>
+      </c>
+      <c r="K26" s="3">
+        <f t="shared" ref="K26" si="50">D26</f>
+        <v>4.99343566095009E-2</v>
+      </c>
+      <c r="L26" s="3">
+        <f t="shared" ref="L26" si="51">E26</f>
+        <v>4.9655528313587799E-2</v>
+      </c>
+      <c r="M26" s="3">
+        <f t="shared" ref="M26" si="52">F26</f>
+        <v>5.17825598545422E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27">
+        <v>1.1478006747407E-2</v>
+      </c>
+      <c r="C27">
+        <v>1.1705198389509199E-2</v>
+      </c>
+      <c r="D27">
+        <v>1.15412959846768E-2</v>
+      </c>
+      <c r="E27">
+        <v>1.16239176444391E-2</v>
+      </c>
+      <c r="F27">
+        <v>1.1311980174596999E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="I8:I11 I7:K7 I5:L5 I3:K3 J10:J11 K11:M11 M5:M6 L7:M7 J9:M9 L10:M10 I4:K4 I6:J6 L6 J8:M8" formula="1"/>
+    <ignoredError sqref="I8:I11 I7:K7 I5:L5 I3:K3 J10:J11 K11:M11 M5:M6 L7:M7 J9:M9 K10:M10 I4:K4 I6:K6 L6 J8:M8 I17:K17 I18:I20 K18:K20 L19:M19 I21:K21 L21:M21 I23:J23 K23:L23 M22:M24 I25:K25 L25:M25 I24:K24 L20:M20 I22:L22 L24 J18:J20" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adjustment of params according to Isabelle. Added her phd thesis and NetLogo code.
</commit_message>
<xml_diff>
--- a/format_aggregate_results.xlsx
+++ b/format_aggregate_results.xlsx
@@ -475,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E3" zoomScale="150" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1003,6 +1003,9 @@
       </c>
       <c r="I13" s="4"/>
     </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J14" s="1"/>
+    </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>0</v>

</xml_diff>